<commit_message>
moved all NI 2Weekly Packages
</commit_message>
<xml_diff>
--- a/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Suite 2WeeklyCatZ201718.xlsx
+++ b/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Suite 2WeeklyCatZ201718.xlsx
@@ -4,20 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="24" windowWidth="14340" windowHeight="4512" activeTab="2"/>
+    <workbookView activeTab="2" windowHeight="4512" windowWidth="14340" xWindow="384" yWindow="24"/>
   </bookViews>
   <sheets>
-    <sheet name="first" sheetId="1" r:id="rId1"/>
-    <sheet name="NI2WeeklyCat_Z" sheetId="2" r:id="rId2"/>
-    <sheet name="ProcessPayrollForNIWeekly" sheetId="4" r:id="rId3"/>
-    <sheet name="TestReports" sheetId="5" r:id="rId4"/>
+    <sheet name="first" r:id="rId1" sheetId="1"/>
+    <sheet name="NI2WeeklyCat_Z" r:id="rId2" sheetId="2"/>
+    <sheet name="ProcessPayrollForNIWeekly" r:id="rId3" sheetId="4"/>
+    <sheet name="TestReports" r:id="rId4" sheetId="5"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="52">
   <si>
     <t>TC</t>
   </si>
@@ -179,6 +179,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -226,68 +227,68 @@
     </border>
   </borders>
   <cellStyleXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="19">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="2">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="2">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="2"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -301,10 +302,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -462,7 +463,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -471,13 +472,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -487,7 +488,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -496,7 +497,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -505,7 +506,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -515,12 +516,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -551,7 +552,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -570,7 +571,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -582,7 +583,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -591,10 +592,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="46.21875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="30.77734375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="33.5546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="46.21875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="30.77734375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="33.5546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.44140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -625,7 +626,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="3" s="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>30</v>
       </c>
@@ -639,7 +640,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row customFormat="1" ht="43.2" r="4" s="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>28</v>
       </c>
@@ -664,7 +665,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row customFormat="1" ht="28.8" r="6" s="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>13</v>
       </c>
@@ -675,7 +676,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+    <row ht="72" r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -687,13 +688,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -702,12 +703,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="82.44140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.77734375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.33203125" style="5" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="7.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="35.109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="82.44140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="14.77734375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="5" width="25.33203125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="7.21875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -858,13 +859,13 @@
       <c r="H8" s="2"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -873,19 +874,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="50.88671875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="35.88671875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="21.21875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.6640625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.88671875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="36.77734375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="42.44140625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="62.109375" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.21875" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="16.88671875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="50.88671875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="35.88671875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="21.21875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="12.6640625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.88671875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="36.77734375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="42.44140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="62.109375" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.21875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="16.88671875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="13" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="27.6" r="1" s="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>32</v>
       </c>
@@ -926,7 +927,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="17" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="27.6" r="2" s="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>50</v>
       </c>
@@ -961,7 +962,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="13" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="27.6" r="3" s="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>50</v>
       </c>
@@ -996,7 +997,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:13" s="13" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="27.6" r="4" s="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>50</v>
       </c>
@@ -1031,7 +1032,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:13" s="13" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="27.6" r="5" s="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>50</v>
       </c>
@@ -1066,7 +1067,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:13" s="13" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="27.6" r="6" s="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>50</v>
       </c>
@@ -1101,7 +1102,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:13" s="13" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="27.6" r="7" s="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
         <v>50</v>
       </c>
@@ -1136,7 +1137,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:13" s="13" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="27.6" r="8" s="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
         <v>50</v>
       </c>
@@ -1173,16 +1174,16 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
-    <hyperlink ref="E3:E8" r:id="rId2" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
+    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId1" ref="E2"/>
+    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId2" ref="E3:E8"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId3" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1191,20 +1192,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="52.88671875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="34.21875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.21875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.77734375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="33.109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="42.88671875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="61.21875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14.44140625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12.21875" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="23.77734375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="52.88671875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="34.21875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="19.109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="15.21875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.77734375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="33.109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="42.88671875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="61.21875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="14.44140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="12.21875" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="23.77734375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="7" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="27.6" r="1" s="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>32</v>
       </c>
@@ -1248,7 +1249,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="11" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="27.6" r="2" s="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>50</v>
       </c>
@@ -1288,8 +1289,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
+    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId1" ref="E2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>